<commit_message>
feat(chamada-new): reativar importação CSV/XLSX com modelos; apenas 'name' obrigatório
</commit_message>
<xml_diff>
--- a/public/templates/students.xlsx
+++ b/public/templates/students.xlsx
@@ -397,47 +397,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>name</v>
-      </c>
-      <c r="B1" t="str">
-        <v>cpf</v>
-      </c>
-      <c r="C1" t="str">
-        <v>contact</v>
+        <v>Atenção: SOMENTE 'name' é obrigatório. 'cpf' e 'contact' são opcionais.</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Maria Silva</v>
+        <v>name</v>
       </c>
       <c r="B2" t="str">
-        <v>000.000.000-00</v>
+        <v>cpf</v>
       </c>
       <c r="C2" t="str">
-        <v>(11) 90000-0000</v>
+        <v>contact</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
+        <v>Maria Silva</v>
+      </c>
+      <c r="B3" t="str">
+        <v>12345678901</v>
+      </c>
+      <c r="C3" t="str">
+        <v>(48) 99999-9999</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
         <v>João Souza</v>
       </c>
-      <c r="B3" t="str">
-        <v>111.111.111-11</v>
-      </c>
-      <c r="C3" t="str">
-        <v>(21) 98888-7777</v>
+      <c r="B4" t="str">
+        <v/>
+      </c>
+      <c r="C4" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>